<commit_message>
Fixed context menu enabling/disabling. Updated formatting of use cases.
</commit_message>
<xml_diff>
--- a/test/use-cases.xlsx
+++ b/test/use-cases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="306">
   <si>
     <t>Action</t>
   </si>
@@ -38,15 +38,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Restart extension in Chrome extensions page</t>
-  </si>
-  <si>
-    <t>No error reported after restart</t>
-  </si>
-  <si>
-    <t>Go to chrome://extensions or click the extension icon in the toolbar and choose "Manage extensions".</t>
-  </si>
-  <si>
     <t>Click the "Details" button for the extension and then click "Extension options" near the bottom of the screen.</t>
   </si>
   <si>
@@ -945,6 +936,12 @@
   </si>
   <si>
     <t>List appears in document, with any other disappearing.</t>
+  </si>
+  <si>
+    <t>Restart Chrome. Go to Manage extensions.</t>
+  </si>
+  <si>
+    <t>Conradish extension does not report any error</t>
   </si>
 </sst>
 </file>
@@ -1017,9 +1014,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1027,14 +1021,395 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <font>
         <name val="Lohit Devanagari"/>
@@ -1774,153 +2149,151 @@
   <dimension ref="A1:AMK12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="45.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="53.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="3" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125" style="4"/>
+    <col min="3" max="3" width="14.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="63.42578125" style="2" customWidth="1"/>
+    <col min="5" max="1025" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="25.5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>304</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>305</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="38.25">
       <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="38.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="25.5">
       <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="25.5">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="25.5">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="51">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4" ht="25.5">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>9</v>
+      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="25.5">
       <c r="A12" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="C12" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C12">
+    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1929,7 +2302,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C11">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C12">
       <formula1>"Pass,Fail,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1947,335 +2320,350 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="45.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="53.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="3" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125" style="4"/>
+    <col min="3" max="3" width="14.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="63.42578125" style="2" customWidth="1"/>
+    <col min="5" max="1025" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="38.25">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>32</v>
+      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="25.5">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>291</v>
+      </c>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>297</v>
+      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="C12" s="6"/>
+        <v>293</v>
+      </c>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="C13" s="6"/>
+        <v>299</v>
+      </c>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="25.5">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="3" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>303</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>305</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>306</v>
-      </c>
+        <v>303</v>
+      </c>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>56</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>65</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>62</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C31" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C16">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C31">
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2284,7 +2672,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C16">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C31">
       <formula1>"Pass,Fail,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2302,379 +2690,410 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="45.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="53.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="3" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125" style="4"/>
+    <col min="3" max="3" width="14.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="63.42578125" style="2" customWidth="1"/>
+    <col min="5" max="1025" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25.5">
       <c r="A2" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="6"/>
+        <v>69</v>
+      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>73</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>75</v>
+      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>76</v>
+      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="6"/>
+        <v>78</v>
+      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>80</v>
+      </c>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="38.25">
       <c r="A9" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="6"/>
+        <v>82</v>
+      </c>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="25.5">
       <c r="A10" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="6"/>
+        <v>84</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>89</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="25.5">
       <c r="A12" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>91</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>93</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="25.5">
       <c r="A14" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>95</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="25.5">
       <c r="A16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" ht="25.5">
+      <c r="A19" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="25.5">
-      <c r="A19" s="1" t="s">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="1" t="s">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" ht="25.5">
+      <c r="A23" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" ht="25.5">
+      <c r="A24" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="25.5">
-      <c r="A23" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="25.5">
-      <c r="A24" s="1" t="s">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" ht="25.5">
+      <c r="A29" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="25.5">
-      <c r="A29" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3" ht="25.5">
+      <c r="A33" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" ht="25.5">
-      <c r="A33" s="1" t="s">
+      <c r="B34" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:3" ht="38.25">
+      <c r="A37" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C37" s="5"/>
+    </row>
+    <row r="38" spans="1:3" ht="25.5">
+      <c r="A38" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="38.25">
-      <c r="A37" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="C38" s="5"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" ht="25.5">
-      <c r="A38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="C39" s="5"/>
+    </row>
+    <row r="40" spans="1:3" ht="38.25">
+      <c r="A40" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="C40" s="5"/>
+    </row>
+    <row r="41" spans="1:3" ht="25.5">
+      <c r="A41" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" ht="38.25">
-      <c r="A40" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="25.5">
-      <c r="A41" s="1" t="s">
-        <v>142</v>
-      </c>
       <c r="B41" s="1" t="s">
-        <v>137</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="C41" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C41">
+    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2683,7 +3102,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C10">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C41">
       <formula1>"Pass,Fail,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2702,244 +3121,256 @@
   <dimension ref="A1:AMK23"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C2" sqref="C2:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="45.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="53.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="3" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125" style="4"/>
+    <col min="3" max="3" width="14.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="63.42578125" style="2" customWidth="1"/>
+    <col min="5" max="1025" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="6"/>
+        <v>70</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="25.5">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C3" s="6"/>
+        <v>142</v>
+      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="25.5">
       <c r="A4" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>144</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="25.5">
       <c r="A5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>147</v>
+      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" s="6"/>
+        <v>150</v>
+      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="25.5">
       <c r="A8" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>152</v>
+      </c>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="C9" s="6"/>
+        <v>162</v>
+      </c>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="25.5">
       <c r="A10" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="C10" s="6"/>
+        <v>154</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>156</v>
+      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="38.25">
       <c r="A12" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>161</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>166</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>166</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="25.5">
       <c r="A15" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>169</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>169</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>292</v>
-      </c>
+      <c r="C23" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C11">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C23">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation operator="equal" allowBlank="1" showErrorMessage="1" sqref="C1">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C11">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C23">
       <formula1>"Pass,Fail,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2957,339 +3388,365 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="45.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="53.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="3" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125" style="4"/>
+    <col min="3" max="3" width="14.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="63.42578125" style="2" customWidth="1"/>
+    <col min="5" max="1025" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25.5">
       <c r="A2" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C2" s="6"/>
+        <v>220</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="C3" s="6"/>
+        <v>222</v>
+      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="25.5">
       <c r="A4" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>224</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="25.5">
       <c r="A5" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>226</v>
+      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>228</v>
+      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C7" s="6"/>
+        <v>229</v>
+      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>232</v>
+      </c>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="C9" s="6"/>
+        <v>235</v>
+      </c>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="25.5">
       <c r="A10" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="C10" s="6"/>
+        <v>226</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>239</v>
-      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="25.5">
       <c r="A12" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>241</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>244</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>245</v>
-      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>247</v>
-      </c>
+        <v>244</v>
+      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" ht="25.5">
+      <c r="A26" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C26" s="5"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="25.5">
-      <c r="A26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C27" s="5"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="C29" s="5"/>
+    </row>
+    <row r="30" spans="1:3" ht="25.5">
+      <c r="A30" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1" t="s">
+      <c r="B30" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" ht="38.25">
+      <c r="A31" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="25.5">
-      <c r="A30" s="1" t="s">
+      <c r="B31" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" ht="38.25">
+      <c r="A32" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="38.25">
-      <c r="A31" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="38.25">
-      <c r="A32" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="C33" s="5"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1" t="s">
+      <c r="B34" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C34" s="5"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="B36" s="1" t="s">
-        <v>277</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="C36" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C36">
+    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3298,7 +3755,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C10">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C36">
       <formula1>"Pass,Fail,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3316,259 +3773,275 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="45.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="53.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="63.42578125" style="3" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125" style="4"/>
+    <col min="3" max="3" width="14.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="63.42578125" style="2" customWidth="1"/>
+    <col min="5" max="1025" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25.5">
       <c r="A2" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="6"/>
+        <v>171</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C3" s="6"/>
+        <v>173</v>
+      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="25.5">
       <c r="A4" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="C4" s="6"/>
+        <v>178</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="C5" s="6"/>
+        <v>176</v>
+      </c>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>179</v>
+      </c>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="C7" s="6"/>
+        <v>181</v>
+      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C8" s="6"/>
+        <v>183</v>
+      </c>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="C9" s="6"/>
+        <v>185</v>
+      </c>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="C10" s="6"/>
+        <v>186</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>192</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>193</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="25.5">
       <c r="A14" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>196</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="25.5">
       <c r="A15" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>199</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C16" s="5"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B19" s="1" t="s">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3" ht="25.5">
+      <c r="A23" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C23" s="5"/>
+    </row>
+    <row r="24" spans="1:3" ht="25.5">
+      <c r="A24" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="25.5">
-      <c r="A23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C24" s="5"/>
+    </row>
+    <row r="25" spans="1:3" ht="51">
+      <c r="A25" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="25.5">
-      <c r="A24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="C25" s="5"/>
+    </row>
+    <row r="26" spans="1:3" ht="25.5">
+      <c r="A26" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="51">
-      <c r="A25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="25.5">
-      <c r="A26" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>221</v>
-      </c>
+      <c r="C26" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C10">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C26">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3577,7 +4050,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C10">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C26">
       <formula1>"Pass,Fail,"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Updated changelog (issue #120). Added test case for copying to Word.
</commit_message>
<xml_diff>
--- a/test/use-cases.xlsx
+++ b/test/use-cases.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="413">
   <si>
     <t>Action</t>
   </si>
@@ -1259,6 +1259,12 @@
   </si>
   <si>
     <t>Use extension in Russian.</t>
+  </si>
+  <si>
+    <t>Copy a paragraph and paste it into Microsoft Word.</t>
+  </si>
+  <si>
+    <t>Text should look correct in Word.</t>
   </si>
 </sst>
 </file>
@@ -2795,21 +2801,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C32">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3108,21 +3114,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C41">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3602,21 +3608,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C41">
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3641,10 +3647,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK32"/>
+  <dimension ref="A1:AMK33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="A32:B32"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3949,23 +3955,31 @@
       </c>
       <c r="C32" s="5"/>
     </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>412</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C32">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4344,21 +4358,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C36">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed font selection when selected font is removed. Minor updates to use cases.
</commit_message>
<xml_diff>
--- a/test/use-cases.xlsx
+++ b/test/use-cases.xlsx
@@ -1398,9 +1398,6 @@
     <t>Go to Manage extensions. Reinstall Conradish extension.</t>
   </si>
   <si>
-    <t>Options page opens in another tab appears.</t>
-  </si>
-  <si>
     <t>Ensure that "Add item to browser context menu", "Filter page content" and "Limit heading size" are checked. Keep options pane open.</t>
   </si>
   <si>
@@ -1474,6 +1471,9 @@
   </si>
   <si>
     <t>Definitions added. Term should be displayed using the correct font.</t>
+  </si>
+  <si>
+    <t>Options page opens in another tab.</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1563,133 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="60">
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF3333"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Lohit Devanagari"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33FF99"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
+    </dxf>
     <dxf>
       <font>
         <name val="Lohit Devanagari"/>
@@ -2555,7 +2681,7 @@
   <dimension ref="A1:AMK23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2595,16 +2721,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>456</v>
+        <v>481</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="38.25">
       <c r="A4" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -2703,93 +2829,102 @@
     </row>
     <row r="15" spans="1:4" ht="25.5">
       <c r="A15" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>459</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>460</v>
-      </c>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="25.5">
       <c r="A16" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:2" ht="25.5">
+    <row r="17" spans="1:3" ht="25.5">
       <c r="A17" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>462</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" ht="25.5">
+      <c r="A18" s="1" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="25.5">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>464</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="5"/>
+    </row>
+    <row r="19" spans="1:3" ht="38.25">
+      <c r="A19" s="1" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="38.25">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>466</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="5"/>
+    </row>
+    <row r="20" spans="1:3" ht="25.5">
+      <c r="A20" s="1" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="25.5">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>468</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="5"/>
+    </row>
+    <row r="21" spans="1:3" ht="25.5">
+      <c r="A21" s="1" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="25.5">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="5"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="1" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="5"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="1" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>474</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>475</v>
-      </c>
+      <c r="C23" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C14">
-    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C23">
+    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2798,7 +2933,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C14">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C23">
       <formula1>"Pass,Fail,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -21428,21 +21563,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C33">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21469,8 +21604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21798,10 +21933,10 @@
     </row>
     <row r="31" spans="1:4" ht="38.25">
       <c r="A31" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
@@ -21834,10 +21969,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C34" s="5"/>
     </row>
@@ -21876,21 +22011,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C37">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21918,7 +22053,7 @@
   <dimension ref="A1:AMK41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22189,21 +22324,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C41">
-    <cfRule type="cellIs" dxfId="44" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="42" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22231,7 +22366,7 @@
   <dimension ref="A1:AMK50"/>
   <sheetViews>
     <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22691,29 +22826,30 @@
     </row>
     <row r="50" spans="1:3" ht="25.5">
       <c r="A50" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>480</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>481</v>
-      </c>
+      <c r="C50" s="5"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C49">
-    <cfRule type="cellIs" dxfId="39" priority="2" operator="equal">
+  <conditionalFormatting sqref="C2:C50">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="37" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22722,7 +22858,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C49">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C50">
       <formula1>"Pass,Fail,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -22741,7 +22877,7 @@
   <dimension ref="A1:AMK36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -41479,21 +41615,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C36">
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="32" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41521,7 +41657,7 @@
   <dimension ref="A1:AMK17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -41693,21 +41829,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41735,7 +41871,7 @@
   <dimension ref="A1:AMK37"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:C37"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -42087,21 +42223,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C37">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42129,7 +42265,7 @@
   <dimension ref="A1:AMK34"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -42454,21 +42590,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C34">
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42496,7 +42632,7 @@
   <dimension ref="A1:AMK33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -61095,21 +61231,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C33">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed usage of lowercase alternative (issue #151).
</commit_message>
<xml_diff>
--- a/test/use-cases.xlsx
+++ b/test/use-cases.xlsx
@@ -372,13 +372,7 @@
     <t>Add definitions in Simplified Chinese.</t>
   </si>
   <si>
-    <t>Definitions in Simplified Chinese appear in footer.</t>
-  </si>
-  <si>
     <t>Add definitions in Traditional Chinese.</t>
-  </si>
-  <si>
-    <t>Definitions in Traditional Chinese appear.</t>
   </si>
   <si>
     <t>Add definition to a word at the beginning of sentence.</t>
@@ -1475,6 +1469,12 @@
   <si>
     <t>Options page opens in another tab.</t>
   </si>
+  <si>
+    <t>Definitions in Simplified Chinese appear in footer. Fonts for footnote should reflect script.</t>
+  </si>
+  <si>
+    <t>Definitions in Traditional Chinese appear. Fonts for footnote should reflect script.</t>
+  </si>
 </sst>
 </file>
 
@@ -1563,133 +1563,7 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="60">
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3333"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33FF99"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3333"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33FF99"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="hair">
-          <color auto="1"/>
-        </left>
-        <right style="hair">
-          <color auto="1"/>
-        </right>
-        <top style="hair">
-          <color auto="1"/>
-        </top>
-        <bottom style="hair">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3333"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33FF99"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF3333"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <name val="Lohit Devanagari"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33FF99"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" shrinkToFit="0"/>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <font>
         <name val="Lohit Devanagari"/>
@@ -2709,10 +2583,10 @@
     </row>
     <row r="2" spans="1:4" ht="25.5">
       <c r="A2" s="1" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -2721,16 +2595,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="38.25">
       <c r="A4" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -2796,7 +2670,7 @@
         <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C11" s="5"/>
     </row>
@@ -2811,10 +2685,10 @@
     </row>
     <row r="13" spans="1:4" ht="25.5">
       <c r="A13" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C13" s="5"/>
     </row>
@@ -2823,22 +2697,22 @@
         <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="25.5">
       <c r="A15" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="25.5">
       <c r="A16" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -2847,84 +2721,84 @@
     </row>
     <row r="17" spans="1:3" ht="25.5">
       <c r="A17" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="25.5">
       <c r="A18" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="38.25">
       <c r="A19" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="25.5">
       <c r="A20" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="25.5">
       <c r="A21" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C23" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C23">
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="57" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2980,85 +2854,85 @@
     </row>
     <row r="2" spans="1:1025">
       <c r="A2" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:1025">
       <c r="A3" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:1025">
       <c r="A4" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:1025">
       <c r="A5" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:1025">
       <c r="A6" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:1025" s="3" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:1025" s="3" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:1025" s="3" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:1025" s="3" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="2"/>
@@ -21563,21 +21437,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C33">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21693,55 +21567,55 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C13" s="5"/>
     </row>
@@ -21807,28 +21681,28 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -21846,10 +21720,10 @@
     </row>
     <row r="23" spans="1:4" ht="25.5">
       <c r="A23" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -21904,7 +21778,7 @@
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -21916,7 +21790,7 @@
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -21928,19 +21802,19 @@
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="38.25">
       <c r="A31" s="1" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -21952,80 +21826,80 @@
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C35" s="5"/>
       <c r="D35" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C37">
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22081,184 +21955,184 @@
     </row>
     <row r="2" spans="1:4" ht="25.5">
       <c r="A2" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="25.5">
       <c r="A5" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="25.5">
       <c r="A10" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="25.5">
       <c r="A16" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="2" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:4" ht="63.75">
       <c r="A19" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:4" ht="38.25">
       <c r="A20" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C21" s="5"/>
     </row>
@@ -22324,21 +22198,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C41">
-    <cfRule type="cellIs" dxfId="49" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="47" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22365,8 +22239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK50"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22559,7 +22433,7 @@
         <v>81</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C20" s="5"/>
     </row>
@@ -22592,7 +22466,7 @@
     </row>
     <row r="24" spans="1:3" ht="25.5">
       <c r="A24" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>66</v>
@@ -22637,10 +22511,10 @@
     </row>
     <row r="29" spans="1:3" ht="25.5">
       <c r="A29" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C29" s="5"/>
     </row>
@@ -22653,108 +22527,108 @@
       </c>
       <c r="C30" s="5"/>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" ht="25.5">
       <c r="A31" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>114</v>
+        <v>480</v>
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" ht="25.5">
       <c r="A32" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>116</v>
+        <v>481</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" ht="25.5">
       <c r="A33" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3" ht="38.25">
       <c r="A37" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="25.5">
       <c r="A38" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" ht="38.25">
       <c r="A40" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" ht="25.5">
       <c r="A41" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" ht="25.5">
       <c r="A42" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>110</v>
@@ -22763,25 +22637,25 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" ht="25.5">
       <c r="A45" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>66</v>
@@ -22790,16 +22664,16 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" ht="25.5">
       <c r="A47" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>66</v>
@@ -22808,48 +22682,48 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C48" s="5"/>
     </row>
     <row r="49" spans="1:3" ht="38.25">
       <c r="A49" s="1" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C49" s="5"/>
     </row>
     <row r="50" spans="1:3" ht="25.5">
       <c r="A50" s="1" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="C50" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C50">
-    <cfRule type="cellIs" dxfId="44" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="42" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -22905,7 +22779,7 @@
     </row>
     <row r="2" spans="1:4" s="3" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
@@ -22915,170 +22789,170 @@
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" ht="25.5">
       <c r="A3" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="25.5">
       <c r="A4" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" s="3" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1" ht="25.5">
       <c r="A10" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" s="3" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" ht="25.5">
       <c r="A13" s="1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" s="3" customFormat="1">
       <c r="A15" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" s="3" customFormat="1">
       <c r="A16" s="1" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:1025" s="3" customFormat="1">
       <c r="A17" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:1025" s="3" customFormat="1">
       <c r="A18" s="1" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:1025" s="2" customFormat="1" ht="25.5">
       <c r="A19" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C19" s="5"/>
       <c r="E19" s="3"/>
@@ -24105,10 +23979,10 @@
     </row>
     <row r="20" spans="1:1025" s="2" customFormat="1">
       <c r="A20" s="1" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C20" s="5"/>
       <c r="E20" s="3"/>
@@ -25135,10 +25009,10 @@
     </row>
     <row r="21" spans="1:1025" s="2" customFormat="1">
       <c r="A21" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C21" s="5"/>
       <c r="E21" s="3"/>
@@ -26165,10 +26039,10 @@
     </row>
     <row r="22" spans="1:1025" s="2" customFormat="1">
       <c r="A22" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C22" s="5"/>
       <c r="E22" s="3"/>
@@ -27195,10 +27069,10 @@
     </row>
     <row r="23" spans="1:1025" s="2" customFormat="1">
       <c r="A23" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C23" s="5"/>
       <c r="E23" s="3"/>
@@ -28225,10 +28099,10 @@
     </row>
     <row r="24" spans="1:1025" s="2" customFormat="1">
       <c r="A24" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C24" s="5"/>
       <c r="E24" s="3"/>
@@ -29255,10 +29129,10 @@
     </row>
     <row r="25" spans="1:1025" s="2" customFormat="1">
       <c r="A25" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C25" s="5"/>
       <c r="E25" s="3"/>
@@ -30285,10 +30159,10 @@
     </row>
     <row r="26" spans="1:1025" s="2" customFormat="1">
       <c r="A26" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C26" s="5"/>
       <c r="E26" s="3"/>
@@ -31315,10 +31189,10 @@
     </row>
     <row r="27" spans="1:1025" s="2" customFormat="1">
       <c r="A27" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C27" s="5"/>
       <c r="E27" s="3"/>
@@ -32345,10 +32219,10 @@
     </row>
     <row r="28" spans="1:1025" s="2" customFormat="1">
       <c r="A28" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C28" s="5"/>
       <c r="E28" s="3"/>
@@ -33375,10 +33249,10 @@
     </row>
     <row r="29" spans="1:1025" s="2" customFormat="1">
       <c r="A29" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C29" s="5"/>
       <c r="E29" s="3"/>
@@ -34405,10 +34279,10 @@
     </row>
     <row r="30" spans="1:1025" s="2" customFormat="1">
       <c r="A30" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C30" s="5"/>
       <c r="E30" s="3"/>
@@ -35435,10 +35309,10 @@
     </row>
     <row r="31" spans="1:1025" s="2" customFormat="1">
       <c r="A31" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C31" s="5"/>
       <c r="E31" s="3"/>
@@ -36465,10 +36339,10 @@
     </row>
     <row r="32" spans="1:1025" s="2" customFormat="1">
       <c r="A32" s="1" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C32" s="5"/>
       <c r="E32" s="3"/>
@@ -37495,10 +37369,10 @@
     </row>
     <row r="33" spans="1:1025" s="2" customFormat="1">
       <c r="A33" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C33" s="5"/>
       <c r="E33" s="3"/>
@@ -38525,10 +38399,10 @@
     </row>
     <row r="34" spans="1:1025" s="2" customFormat="1">
       <c r="A34" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C34" s="5"/>
       <c r="E34" s="3"/>
@@ -39555,10 +39429,10 @@
     </row>
     <row r="35" spans="1:1025" s="2" customFormat="1">
       <c r="A35" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C35" s="5"/>
       <c r="E35" s="3"/>
@@ -40585,10 +40459,10 @@
     </row>
     <row r="36" spans="1:1025" s="2" customFormat="1">
       <c r="A36" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C36" s="5"/>
       <c r="E36" s="3"/>
@@ -41615,21 +41489,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C36">
-    <cfRule type="cellIs" dxfId="39" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="37" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41685,7 +41559,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>66</v>
@@ -41694,156 +41568,156 @@
     </row>
     <row r="3" spans="1:4" ht="25.5">
       <c r="A3" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="25.5">
       <c r="A4" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="25.5">
       <c r="A5" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="25.5">
       <c r="A8" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="25.5">
       <c r="A10" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="38.25">
       <c r="A12" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="25.5">
       <c r="A15" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="C17" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -41899,345 +41773,345 @@
     </row>
     <row r="2" spans="1:4" ht="25.5">
       <c r="A2" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="25.5">
       <c r="A4" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="25.5">
       <c r="A5" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4" ht="25.5">
       <c r="A10" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:4" ht="25.5">
       <c r="A12" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="25.5">
       <c r="A26" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" ht="25.5">
       <c r="A30" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" ht="38.25">
       <c r="A31" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" ht="38.25">
       <c r="A32" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="1" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C37" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C37">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42293,88 +42167,88 @@
     </row>
     <row r="2" spans="1:4" ht="25.5">
       <c r="A2" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="25.5">
       <c r="A4" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="38.25">
       <c r="A7" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -42383,228 +42257,228 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:4" ht="25.5">
       <c r="A14" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:4" ht="25.5">
       <c r="A15" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" ht="25.5">
       <c r="A23" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" ht="25.5">
       <c r="A24" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" ht="51">
       <c r="A25" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="25.5">
       <c r="A27" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" ht="25.5">
       <c r="A29" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" ht="25.5">
       <c r="A33" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" ht="25.5">
       <c r="A34" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C34" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C34">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="3" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42660,55 +42534,55 @@
     </row>
     <row r="2" spans="1:1025">
       <c r="A2" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:1025">
       <c r="A3" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:1025">
       <c r="A4" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:1025">
       <c r="A5" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:1025">
       <c r="A6" s="1" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:1025" s="3" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="2"/>
@@ -61231,21 +61105,21 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C33">
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Opening user guide on install. Updated use cases.
</commit_message>
<xml_diff>
--- a/test/use-cases.xlsx
+++ b/test/use-cases.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="480">
   <si>
     <t>Action</t>
   </si>
@@ -1164,22 +1164,10 @@
     <t>Open new English article. Choose Arabic as the "to" language.</t>
   </si>
   <si>
-    <t>Open Hebrew article. Choose Polish as the "to" language.</t>
-  </si>
-  <si>
     <t>Add definitions to words.</t>
   </si>
   <si>
-    <t>Switch "to" language to Arabic. Add definitions until their number exceeds the number of English definitions.</t>
-  </si>
-  <si>
     <t>Definitions added. Footer aligns to the right.</t>
-  </si>
-  <si>
-    <t>Definitions added. Footer aligns to the left.</t>
-  </si>
-  <si>
-    <t>Footer now aligns to the right.</t>
   </si>
   <si>
     <t>Document is listed under new title.</t>
@@ -1461,9 +1449,6 @@
     <t>Text should look right.</t>
   </si>
   <si>
-    <t>Open Urdu article. Add definitions to words.</t>
-  </si>
-  <si>
     <t>Definitions added. Term should be displayed using the correct font.</t>
   </si>
   <si>
@@ -1474,6 +1459,15 @@
   </si>
   <si>
     <t>Definitions in Traditional Chinese appear. Fonts for footnote should reflect script.</t>
+  </si>
+  <si>
+    <t>Open Urdu article. Add definitions to words. Choose Polish as the "to" language.</t>
+  </si>
+  <si>
+    <t>Use extension in Chinese (Simplified)</t>
+  </si>
+  <si>
+    <t>Use extension in Chinese (Traditional)</t>
   </si>
 </sst>
 </file>
@@ -2583,7 +2577,7 @@
     </row>
     <row r="2" spans="1:4" ht="25.5">
       <c r="A2" s="1" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>294</v>
@@ -2595,16 +2589,16 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="38.25">
       <c r="A4" s="1" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -2703,16 +2697,16 @@
     </row>
     <row r="15" spans="1:4" ht="25.5">
       <c r="A15" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="25.5">
       <c r="A16" s="1" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -2721,64 +2715,64 @@
     </row>
     <row r="17" spans="1:3" ht="25.5">
       <c r="A17" s="1" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="25.5">
       <c r="A18" s="1" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="38.25">
       <c r="A19" s="1" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="25.5">
       <c r="A20" s="1" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="25.5">
       <c r="A21" s="1" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C23" s="5"/>
     </row>
@@ -2826,7 +2820,7 @@
   <dimension ref="A1:AMK33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2854,98 +2848,106 @@
     </row>
     <row r="2" spans="1:1025">
       <c r="A2" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:1025">
       <c r="A3" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:1025">
       <c r="A4" s="1" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:1025">
       <c r="A5" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:1025">
       <c r="A6" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:1025" s="3" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:1025" s="3" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:1025" s="3" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:1025" s="3" customFormat="1">
       <c r="A10" s="1" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:1025" s="3" customFormat="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>412</v>
+      </c>
       <c r="C11" s="5"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:1025" s="3" customFormat="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>412</v>
+      </c>
       <c r="C12" s="5"/>
       <c r="D12" s="2"/>
     </row>
@@ -21478,8 +21480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -21807,10 +21809,10 @@
     </row>
     <row r="31" spans="1:4" ht="38.25">
       <c r="A31" s="1" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="2" t="s">
@@ -21843,10 +21845,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C34" s="5"/>
     </row>
@@ -21927,7 +21929,7 @@
   <dimension ref="A1:AMK41"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22237,10 +22239,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK50"/>
+  <dimension ref="A1:AMK47"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31:B32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22532,7 +22534,7 @@
         <v>113</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="C31" s="5"/>
     </row>
@@ -22541,7 +22543,7 @@
         <v>114</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="C32" s="5"/>
     </row>
@@ -22664,51 +22666,24 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="C46" s="5"/>
     </row>
     <row r="47" spans="1:3" ht="25.5">
       <c r="A47" s="1" t="s">
-        <v>378</v>
+        <v>477</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>66</v>
+        <v>473</v>
       </c>
       <c r="C47" s="5"/>
     </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C48" s="5"/>
-    </row>
-    <row r="49" spans="1:3" ht="38.25">
-      <c r="A49" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C49" s="5"/>
-    </row>
-    <row r="50" spans="1:3" ht="25.5">
-      <c r="A50" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="C50" s="5"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C50">
+  <conditionalFormatting sqref="C2:C47">
     <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
@@ -22732,7 +22707,7 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C50">
+    <dataValidation type="list" operator="equal" allowBlank="1" showErrorMessage="1" sqref="C2:C47">
       <formula1>"Pass,Fail,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -22751,7 +22726,7 @@
   <dimension ref="A1:AMK36"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -22789,170 +22764,170 @@
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" ht="25.5">
       <c r="A3" s="1" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" ht="25.5">
       <c r="A4" s="1" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1">
       <c r="A5" s="1" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" s="3" customFormat="1">
       <c r="A6" s="1" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" s="3" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" s="3" customFormat="1">
       <c r="A8" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" s="3" customFormat="1">
       <c r="A9" s="1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" s="3" customFormat="1" ht="25.5">
       <c r="A10" s="1" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" s="3" customFormat="1">
       <c r="A11" s="1" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" s="3" customFormat="1">
       <c r="A12" s="1" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" s="3" customFormat="1" ht="25.5">
       <c r="A13" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1">
       <c r="A14" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" s="3" customFormat="1">
       <c r="A15" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" s="3" customFormat="1">
       <c r="A16" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:1025" s="3" customFormat="1">
       <c r="A17" s="1" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:1025" s="3" customFormat="1">
       <c r="A18" s="1" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:1025" s="2" customFormat="1" ht="25.5">
       <c r="A19" s="1" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C19" s="5"/>
       <c r="E19" s="3"/>
@@ -35309,7 +35284,7 @@
     </row>
     <row r="31" spans="1:1025" s="2" customFormat="1">
       <c r="A31" s="1" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>311</v>
@@ -40459,10 +40434,10 @@
     </row>
     <row r="36" spans="1:1025" s="2" customFormat="1">
       <c r="A36" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C36" s="5"/>
       <c r="E36" s="3"/>
@@ -41531,7 +41506,7 @@
   <dimension ref="A1:AMK17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -41694,10 +41669,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C17" s="5"/>
     </row>
@@ -41744,8 +41719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -42138,8 +42113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AMK34"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -42392,64 +42367,64 @@
     </row>
     <row r="27" spans="1:3" ht="25.5">
       <c r="A27" s="1" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="1" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" ht="25.5">
       <c r="A29" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="1" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" ht="25.5">
       <c r="A33" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C33" s="5"/>
     </row>
@@ -42506,7 +42481,7 @@
   <dimension ref="A1:AMK33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -42534,34 +42509,34 @@
     </row>
     <row r="2" spans="1:1025">
       <c r="A2" s="1" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:1025">
       <c r="A3" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:1025">
       <c r="A4" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:1025">
       <c r="A5" s="1" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>191</v>
@@ -42570,19 +42545,19 @@
     </row>
     <row r="6" spans="1:1025">
       <c r="A6" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:1025" s="3" customFormat="1">
       <c r="A7" s="1" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="2"/>

</xml_diff>

<commit_message>
Updated use cases (issue #164).
</commit_message>
<xml_diff>
--- a/test/use-cases.xlsx
+++ b/test/use-cases.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="486">
   <si>
     <t>Action</t>
   </si>
@@ -1468,6 +1468,24 @@
   </si>
   <si>
     <t>Use extension in Chinese (Traditional)</t>
+  </si>
+  <si>
+    <t>Copy a article with footnotes and paste it into Microsoft Word.</t>
+  </si>
+  <si>
+    <t>Text should look correct in Word. Footnotes should be copied.</t>
+  </si>
+  <si>
+    <t>Copy a article with footnotes in Arabic and paste it into Microsoft Word.</t>
+  </si>
+  <si>
+    <t>Text should look correct in Word. Footnotes should be right aligned.</t>
+  </si>
+  <si>
+    <t>Copy a article with footnotes and paste it text editor.</t>
+  </si>
+  <si>
+    <t>Text should look correct. Footnotes should appear at bottom.</t>
   </si>
 </sst>
 </file>
@@ -41503,7 +41521,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK17"/>
+  <dimension ref="A1:AMK19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
@@ -41667,14 +41685,30 @@
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" ht="25.5">
       <c r="A17" s="1" t="s">
-        <v>398</v>
+        <v>480</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>399</v>
+        <v>481</v>
       </c>
       <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" ht="25.5">
+      <c r="A18" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>485</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">

</xml_diff>